<commit_message>
Formatting changes to the Q and A excel
</commit_message>
<xml_diff>
--- a/data/sample_Q_and_A.xlsx
+++ b/data/sample_Q_and_A.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinay.soni\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Code_templates\NLP\hack_in_a_box\ms_hack_in_a_box_202403\code\ai-build\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{011FCD1D-81E3-4515-8DE5-8731E2F81A84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7432982-CD20-481E-B000-FD8083D780A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{5818D820-8763-4836-89B6-125FFE14DA23}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5818D820-8763-4836-89B6-125FFE14DA23}"/>
   </bookViews>
   <sheets>
-    <sheet name="QA" sheetId="1" r:id="rId1"/>
+    <sheet name="Sample q and a" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sample q and a'!$B$2:$C$12</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -108,7 +111,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,20 +120,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -162,10 +176,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,109 +514,113 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17428C67-0FD3-448B-865C-1FD8A3C77455}">
-  <dimension ref="B5:C15"/>
+  <sheetPr>
+    <tabColor theme="7" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="B2:C12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" customWidth="1"/>
-    <col min="2" max="2" width="58.140625" customWidth="1"/>
-    <col min="3" max="3" width="48.28515625" customWidth="1"/>
-    <col min="4" max="4" width="4.5703125" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="2" max="2" width="57.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="1" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="B2:C12" xr:uid="{17428C67-0FD3-448B-865C-1FD8A3C77455}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added SNo in the Q and A excel
</commit_message>
<xml_diff>
--- a/data/sample_Q_and_A.xlsx
+++ b/data/sample_Q_and_A.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Code_templates\NLP\hack_in_a_box\ms_hack_in_a_box_202403\code\ai-build\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7432982-CD20-481E-B000-FD8083D780A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C286A03-1431-4D84-A04A-4A93A647CD8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5818D820-8763-4836-89B6-125FFE14DA23}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5818D820-8763-4836-89B6-125FFE14DA23}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample q and a" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sample q and a'!$B$2:$C$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sample q and a'!$B$2:$D$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Up to 45% by 2050.</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>Question</t>
+  </si>
+  <si>
+    <t>S No</t>
   </si>
 </sst>
 </file>
@@ -517,110 +520,144 @@
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="B2:C12"/>
+  <dimension ref="B2:D12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" customWidth="1"/>
-    <col min="2" max="2" width="57.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.5546875" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B4" s="1" t="s">
+    <row r="4" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B5" s="1" t="s">
+    <row r="5" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B6" s="1" t="s">
+    <row r="6" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B7" s="1" t="s">
+    <row r="7" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B8" s="1" t="s">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B9" s="1" t="s">
+    <row r="9" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B10" s="1" t="s">
+    <row r="10" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="1" t="s">
+    <row r="11" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B12" s="1" t="s">
+    <row r="12" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B2:C12" xr:uid="{17428C67-0FD3-448B-865C-1FD8A3C77455}"/>
+  <autoFilter ref="B2:D12" xr:uid="{17428C67-0FD3-448B-865C-1FD8A3C77455}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added SNo in Q and A excel
</commit_message>
<xml_diff>
--- a/data/sample_Q_and_A.xlsx
+++ b/data/sample_Q_and_A.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Code_templates\NLP\hack_in_a_box\ms_hack_in_a_box_202403\code\ai-build\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C286A03-1431-4D84-A04A-4A93A647CD8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F62E0549-3FAB-417F-B394-16B568E1CE1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5818D820-8763-4836-89B6-125FFE14DA23}"/>
   </bookViews>
@@ -523,7 +523,7 @@
   <dimension ref="B2:D12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,5 +659,6 @@
   </sheetData>
   <autoFilter ref="B2:D12" xr:uid="{17428C67-0FD3-448B-865C-1FD8A3C77455}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>